<commit_message>
Updated and Final Project Schedule
</commit_message>
<xml_diff>
--- a/FinalProjectSchedule.xlsx
+++ b/FinalProjectSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/sakamoto_ca_northeastern_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EACFB9B7-B91B-4721-B801-7C7372784184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D3DFD82-C6D4-43EC-8E78-82B3656BE14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="1572" windowWidth="23016" windowHeight="13656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>PROJECT SCHEDULE</t>
   </si>
@@ -68,9 +68,6 @@
     <t>OVERALL PROGRESS</t>
   </si>
   <si>
-    <t>0%</t>
-  </si>
-  <si>
     <t>TASK NAME</t>
   </si>
   <si>
@@ -170,12 +167,6 @@
     <t>UI: Editing &amp; Autosave</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Autosave after 500 ms idle</t>
-  </si>
-  <si>
     <t>Storage: Notes + Metadata</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>Usability Polish &amp; Accessibility</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Labels, shortcuts</t>
   </si>
   <si>
@@ -255,13 +243,16 @@
   </si>
   <si>
     <t>Contingency, final fixes</t>
+  </si>
+  <si>
+    <t>Autosave after 800 ms idle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +286,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,18 +329,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -363,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -375,17 +354,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,39 +664,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1"/>
@@ -729,7 +705,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -737,15 +713,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -756,23 +732,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="13">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="10">
         <v>45922</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>45989</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -781,589 +757,589 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>45922</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>45923</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="11">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9">
         <v>45924</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>45926</v>
       </c>
       <c r="E9" s="7">
         <v>3</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>45927</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>45929</v>
       </c>
       <c r="E10" s="7">
         <v>3</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15">
-      <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="11">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9">
         <v>45930</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>45934</v>
       </c>
       <c r="E11" s="7">
         <v>5</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15">
-      <c r="A12" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="11">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9">
         <v>45935</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>45949</v>
       </c>
       <c r="E12" s="7">
         <v>15</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15">
-      <c r="A13" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="11">
+        <v>22</v>
+      </c>
+      <c r="C13" s="9">
         <v>45935</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>45946</v>
       </c>
       <c r="E13" s="7">
         <v>12</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15">
-      <c r="A14" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="11">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9">
         <v>45943</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>45955</v>
       </c>
       <c r="E14" s="7">
         <v>13</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="11">
+      <c r="C15" s="9">
         <v>45937</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>45951</v>
       </c>
       <c r="E15" s="7">
         <v>15</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>45942</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>45956</v>
       </c>
       <c r="E16" s="7">
         <v>15</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15">
-      <c r="A17" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="B17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="11">
+        <v>33</v>
+      </c>
+      <c r="C17" s="9">
         <v>45946</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>45960</v>
       </c>
       <c r="E17" s="7">
         <v>15</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="11">
+        <v>36</v>
+      </c>
+      <c r="C18" s="9">
         <v>45940</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>45948</v>
       </c>
       <c r="E18" s="7">
         <v>9</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="11">
+        <v>36</v>
+      </c>
+      <c r="C19" s="9">
         <v>45948</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>45962</v>
       </c>
       <c r="E19" s="7">
         <v>15</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>44</v>
+      <c r="F19" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="11">
+        <v>22</v>
+      </c>
+      <c r="C20" s="9">
         <v>45948</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>45962</v>
       </c>
       <c r="E20" s="7">
         <v>15</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
         <v>44</v>
       </c>
-      <c r="G20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>45952</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>45966</v>
       </c>
       <c r="E21" s="7">
         <v>15</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>44</v>
+      <c r="F21" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="11">
+        <v>36</v>
+      </c>
+      <c r="C22" s="9">
         <v>45956</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>45968</v>
       </c>
       <c r="E22" s="7">
         <v>13</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>44</v>
+      <c r="F22" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="11">
+        <v>36</v>
+      </c>
+      <c r="C23" s="9">
         <v>45960</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>45969</v>
       </c>
       <c r="E23" s="7">
         <v>10</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>44</v>
+      <c r="F23" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="11">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9">
         <v>45991</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>45972</v>
       </c>
       <c r="E24" s="7">
         <v>13</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>44</v>
+      <c r="F24" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="11">
+        <v>33</v>
+      </c>
+      <c r="C25" s="9">
         <v>45963</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>45976</v>
       </c>
       <c r="E25" s="7">
         <v>14</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>44</v>
+      <c r="F25" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="11">
+        <v>16</v>
+      </c>
+      <c r="C26" s="9">
         <v>45970</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>45979</v>
       </c>
       <c r="E26" s="7">
         <v>10</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>59</v>
+      <c r="F26" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="11">
+        <v>36</v>
+      </c>
+      <c r="C27" s="9">
         <v>45972</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>45982</v>
       </c>
       <c r="E27" s="7">
         <v>11</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="B28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="11">
+        <v>16</v>
+      </c>
+      <c r="C28" s="9">
         <v>45978</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>45984</v>
       </c>
       <c r="E28" s="7">
         <v>7</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>59</v>
+      <c r="F28" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="11">
+        <v>16</v>
+      </c>
+      <c r="C29" s="9">
         <v>45979</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>45986</v>
       </c>
       <c r="E29" s="7">
         <v>8</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>59</v>
+      <c r="F29" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="11">
+        <v>16</v>
+      </c>
+      <c r="C30" s="9">
         <v>45966</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>45970</v>
       </c>
       <c r="E30" s="7">
         <v>5</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>59</v>
+      <c r="F30" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="11">
+        <v>16</v>
+      </c>
+      <c r="C31" s="9">
         <v>45981</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>45985</v>
       </c>
       <c r="E31" s="7">
         <v>5</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>59</v>
+      <c r="F31" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="11">
+        <v>16</v>
+      </c>
+      <c r="C32" s="9">
         <v>45985</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>45989</v>
       </c>
       <c r="E32" s="7">
         <v>5</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>59</v>
+      <c r="F32" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1371,10 +1347,6 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1385,14 +1357,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e3a93bbf-f867-4e9c-9600-5e25096a6882" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034FBA4E13F457A4DA1D4BCB199603BFC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="38023e486b0434a9db43ac1c9a783be3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e3a93bbf-f867-4e9c-9600-5e25096a6882" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06a26a2bde8cd33084d2e3961cf4c880" ns3:_="">
     <xsd:import namespace="e3a93bbf-f867-4e9c-9600-5e25096a6882"/>
@@ -1580,6 +1544,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e3a93bbf-f867-4e9c-9600-5e25096a6882" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1590,15 +1562,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917D9143-7C0D-4E73-967D-0B64F9E439B4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{286DF9BC-498E-4868-ADE0-3719C2579E61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e3a93bbf-f867-4e9c-9600-5e25096a6882"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{286DF9BC-498E-4868-ADE0-3719C2579E61}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917D9143-7C0D-4E73-967D-0B64F9E439B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3a93bbf-f867-4e9c-9600-5e25096a6882"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B53E1E4-423E-4AFD-9B8D-F27B26BC535B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B53E1E4-423E-4AFD-9B8D-F27B26BC535B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>